<commit_message>
Se modifica estrategia para prueba automatizada servicio Delete Post
</commit_message>
<xml_diff>
--- a/Plan-de-Calidad.xlsx
+++ b/Plan-de-Calidad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\IdeaProjects\sofka\C1-2023-QA-Auto-ScreenPlay-Rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5CD94-9E55-478B-8DF3-1C146586E443}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF5580E-F5D3-4F74-93AC-C6F0C477B11E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,6 +337,7 @@
         <sz val="11"/>
         <color rgb="FF0563C1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://api.coingecko.com/api/v3/exchanges/{gdax</t>
     </r>
@@ -345,6 +346,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>}</t>
     </r>
@@ -524,6 +526,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Hace parte del alcance</t>
     </r>
@@ -532,6 +535,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">:
 </t>
@@ -542,6 +546,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>-Para el servicio GetExhanges:</t>
     </r>
@@ -550,6 +555,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 *Verificar que se pueda ver la información de los mercados de intercambio de criptomonedas, filtrandolo por su id
@@ -570,6 +576,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 *Verificar que se pueda visualizar la información de las compañias publicas que realizan movimientos en el mercado de criptomonedas, filtrandolas por su id
@@ -591,6 +598,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Hace parte del alcance:    </t>
     </r>
@@ -599,6 +607,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 - Para el servicio Delete Post:</t>
@@ -621,6 +630,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Para los servicios REST de la pagina </t>
     </r>
@@ -630,6 +640,7 @@
         <sz val="11"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.coingecko.com/en/api/documentation</t>
     </r>
@@ -638,6 +649,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> mencionados en el alcance, se implementara la siguiente estrategia.
 1. Realizar pruebas exploratorias para conocer el funcionamiento de los servicios planteados.
@@ -667,6 +679,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">:
 - Los factores no funcionales como el rendimiento, la seguridad informática, la usabilidad, la escalabilidad, etc, no se probaran en este proceso de prueba.
@@ -676,11 +689,11 @@
     </r>
   </si>
   <si>
-    <t>Para los servicios REST de la pagina JsonPlaceHolder
+    <t>Para el servicio REST de la pagina JsonPlaceHolder
 mencionados en el alcance, se implementara la siguiente estrategia.
 1. Realizar pruebas exploratorias para conocer el funcionamiento de los servicios planteados.
-2. Crear escenarios en los cuales los servicios listen la información de manera exitosa (happy path)
-3. Comparar el código de status esperado con el código retornado por los servicios. 
+2. Crear un escenario en el cual el servicio liste la información de manera exitosa (happy path).
+3. Comparar el código de status esperado con el código retornado por el servicio.
 5. Utilizar herramientas de automatización de pruebas para ejecutar los escenarios de prueba creados y validar que los resultados obtenidos sean los esperados.</t>
   </si>
 </sst>
@@ -688,7 +701,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -706,67 +719,79 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -779,32 +804,29 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1191,6 +1213,21 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1206,21 +1243,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2007,9 +2029,9 @@
   </sheetPr>
   <dimension ref="A1:X992"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2034,7 +2056,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="55" t="s">
         <v>114</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -2082,19 +2104,19 @@
       <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="H2" s="51" t="s">
         <v>158</v>
       </c>
       <c r="I2" s="8" t="s">
@@ -2128,19 +2150,19 @@
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="51" t="s">
         <v>163</v>
       </c>
       <c r="G3" s="67" t="s">
         <v>164</v>
       </c>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="51" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="9" t="s">
@@ -27924,82 +27946,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A1" s="51"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="53"/>
+      <c r="A1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A2" s="54"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="61"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="61"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="56"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
     </row>
     <row r="5" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="56"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="61"/>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A6" s="57"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="64"/>
     </row>
     <row r="7" spans="1:11" ht="27" customHeight="1">
       <c r="A7" s="10" t="s">
@@ -41755,10 +41777,10 @@
       <c r="L1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="60" t="s">
+      <c r="N1" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="61"/>
+      <c r="O1" s="66"/>
     </row>
     <row r="2" spans="1:15" ht="14.25" customHeight="1">
       <c r="A2" s="14" t="s">

</xml_diff>